<commit_message>
latest updates to profiles
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-fs.xlsx
+++ b/build/output/StructureDefinition-pacio-fs.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$52</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1907" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="422">
   <si>
     <t>Path</t>
   </si>
@@ -328,33 +328,66 @@
     <t>Observation.extension</t>
   </si>
   <si>
+    <t xml:space="preserve">Extension
+</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>An Extension</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value:url}
+</t>
+  </si>
+  <si>
+    <t>open</t>
+  </si>
+  <si>
+    <t>DomainResource.extension</t>
+  </si>
+  <si>
+    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
+ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
+  </si>
+  <si>
+    <t>event-location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {event-location}
+</t>
+  </si>
+  <si>
+    <t>Where event occurred</t>
+  </si>
+  <si>
+    <t>The principal physical location where the {{title}} was performed.</t>
+  </si>
+  <si>
+    <t>May reference only *Provenance* resources deemed “relevant” or important. This element does not point to the Provenance associated with the current version of the resource - as it would be created after this version existed. The Provenance for the current version can be retrieved with a [` _revinclude`](search.html#revinclude).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ele-1
+</t>
+  </si>
+  <si>
+    <t>Event.location</t>
+  </si>
+  <si>
+    <t>EVN.7</t>
+  </si>
+  <si>
+    <t>.participation[typeCode=LOC].role</t>
+  </si>
+  <si>
+    <t>Observation.modifierExtension</t>
+  </si>
+  <si>
     <t>extensions
 user content</t>
   </si>
   <si>
-    <t xml:space="preserve">Extension
-</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
-  </si>
-  <si>
-    <t>DomainResource.extension</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-ext-1:Must have either extensions or value[x], not both {extension.exists() != value.exists()}</t>
-  </si>
-  <si>
-    <t>Observation.modifierExtension</t>
-  </si>
-  <si>
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
@@ -362,6 +395,9 @@
 Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
+    <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
+  </si>
+  <si>
     <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://hl7.org/fhir/R4/extensibility.html#modifierExtension).</t>
   </si>
   <si>
@@ -1024,6 +1060,9 @@
   </si>
   <si>
     <t>Observation.referenceRange.extension</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
   </si>
   <si>
     <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
@@ -1449,7 +1488,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO51"/>
+  <dimension ref="A1:AO52"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1459,7 +1498,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.1328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.9921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -2449,7 +2488,7 @@
       </c>
       <c r="B9" s="2"/>
       <c r="C9" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" t="s" s="2">
@@ -2468,17 +2507,15 @@
         <v>45</v>
       </c>
       <c r="J9" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K9" t="s" s="2">
         <v>101</v>
       </c>
-      <c r="K9" t="s" s="2">
+      <c r="L9" t="s" s="2">
         <v>102</v>
       </c>
-      <c r="L9" t="s" s="2">
-        <v>103</v>
-      </c>
-      <c r="M9" t="s" s="2">
-        <v>104</v>
-      </c>
+      <c r="M9" s="2"/>
       <c r="N9" s="2"/>
       <c r="O9" t="s" s="2">
         <v>45</v>
@@ -2515,16 +2552,14 @@
         <v>45</v>
       </c>
       <c r="AA9" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB9" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="AB9" s="2"/>
       <c r="AC9" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AD9" t="s" s="2">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="AE9" t="s" s="2">
         <v>105</v>
@@ -2551,7 +2586,7 @@
         <v>45</v>
       </c>
       <c r="AM9" t="s" s="2">
-        <v>98</v>
+        <v>45</v>
       </c>
       <c r="AN9" t="s" s="2">
         <v>45</v>
@@ -2560,45 +2595,45 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" hidden="true">
+    <row r="10">
       <c r="A10" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s" s="2">
         <v>107</v>
       </c>
-      <c r="B10" s="2"/>
       <c r="C10" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G10" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H10" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s" s="2">
         <v>45</v>
       </c>
       <c r="J10" t="s" s="2">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="K10" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L10" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="M10" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N10" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="N10" s="2"/>
       <c r="O10" t="s" s="2">
         <v>45</v>
       </c>
@@ -2646,7 +2681,7 @@
         <v>45</v>
       </c>
       <c r="AE10" t="s" s="2">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="AF10" t="s" s="2">
         <v>43</v>
@@ -2655,22 +2690,22 @@
         <v>44</v>
       </c>
       <c r="AH10" t="s" s="2">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="AI10" t="s" s="2">
         <v>106</v>
       </c>
       <c r="AJ10" t="s" s="2">
-        <v>45</v>
+        <v>113</v>
       </c>
       <c r="AK10" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL10" t="s" s="2">
-        <v>45</v>
+        <v>114</v>
       </c>
       <c r="AM10" t="s" s="2">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="AN10" t="s" s="2">
         <v>45</v>
@@ -2681,11 +2716,11 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2698,23 +2733,25 @@
         <v>45</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I11" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="K11" t="s" s="2">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="L11" t="s" s="2">
-        <v>115</v>
-      </c>
-      <c r="M11" s="2"/>
+        <v>119</v>
+      </c>
+      <c r="M11" t="s" s="2">
+        <v>120</v>
+      </c>
       <c r="N11" t="s" s="2">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="O11" t="s" s="2">
         <v>45</v>
@@ -2763,7 +2800,7 @@
         <v>45</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>43</v>
@@ -2775,22 +2812,22 @@
         <v>45</v>
       </c>
       <c r="AI11" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ11" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="AK11" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL11" t="s" s="2">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="AM11" t="s" s="2">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="AN11" t="s" s="2">
-        <v>120</v>
+        <v>45</v>
       </c>
       <c r="AO11" t="s" s="2">
         <v>45</v>
@@ -2798,11 +2835,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>122</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
@@ -2821,17 +2858,17 @@
         <v>56</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" t="s" s="2">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="O12" t="s" s="2">
         <v>45</v>
@@ -2880,7 +2917,7 @@
         <v>45</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>43</v>
@@ -2895,19 +2932,19 @@
         <v>67</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>45</v>
+        <v>131</v>
       </c>
       <c r="AO12" t="s" s="2">
         <v>45</v>
@@ -2915,11 +2952,11 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
@@ -2938,18 +2975,18 @@
         <v>56</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="M13" t="s" s="2">
-        <v>135</v>
-      </c>
-      <c r="N13" s="2"/>
+        <v>136</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" t="s" s="2">
+        <v>137</v>
+      </c>
       <c r="O13" t="s" s="2">
         <v>45</v>
       </c>
@@ -2997,7 +3034,7 @@
         <v>45</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>43</v>
@@ -3012,16 +3049,16 @@
         <v>67</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>45</v>
@@ -3032,43 +3069,41 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I14" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>75</v>
+        <v>143</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>142</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>143</v>
-      </c>
+        <v>146</v>
+      </c>
+      <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
         <v>45</v>
       </c>
@@ -3092,13 +3127,13 @@
         <v>45</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>144</v>
+        <v>45</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>45</v>
@@ -3116,13 +3151,13 @@
         <v>45</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG14" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH14" t="s" s="2">
         <v>45</v>
@@ -3134,16 +3169,16 @@
         <v>147</v>
       </c>
       <c r="AK14" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL14" t="s" s="2">
         <v>148</v>
       </c>
-      <c r="AL14" t="s" s="2">
+      <c r="AM14" t="s" s="2">
         <v>149</v>
       </c>
-      <c r="AM14" t="s" s="2">
-        <v>150</v>
-      </c>
       <c r="AN14" t="s" s="2">
-        <v>151</v>
+        <v>45</v>
       </c>
       <c r="AO14" t="s" s="2">
         <v>45</v>
@@ -3151,7 +3186,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3159,34 +3194,34 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I15" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J15" t="s" s="2">
+        <v>75</v>
+      </c>
+      <c r="K15" t="s" s="2">
+        <v>151</v>
+      </c>
+      <c r="L15" t="s" s="2">
+        <v>152</v>
+      </c>
+      <c r="M15" t="s" s="2">
         <v>153</v>
       </c>
-      <c r="K15" t="s" s="2">
+      <c r="N15" t="s" s="2">
         <v>154</v>
-      </c>
-      <c r="L15" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>156</v>
-      </c>
-      <c r="N15" t="s" s="2">
-        <v>157</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>45</v>
@@ -3211,13 +3246,13 @@
         <v>45</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>79</v>
+        <v>155</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3235,13 +3270,13 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>45</v>
@@ -3250,19 +3285,19 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>45</v>
+        <v>158</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3270,18 +3305,18 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>163</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>45</v>
@@ -3290,22 +3325,22 @@
         <v>45</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M16" t="s" s="2">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="N16" t="s" s="2">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3330,11 +3365,13 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="X16" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="X16" t="s" s="2">
+        <v>169</v>
+      </c>
       <c r="Y16" t="s" s="2">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3352,13 +3389,13 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>45</v>
@@ -3367,31 +3404,31 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="AL16" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM16" t="s" s="2">
         <v>171</v>
       </c>
-      <c r="AM16" t="s" s="2">
+      <c r="AN16" t="s" s="2">
         <v>172</v>
       </c>
-      <c r="AN16" t="s" s="2">
-        <v>173</v>
-      </c>
       <c r="AO16" t="s" s="2">
-        <v>174</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>45</v>
+        <v>174</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3410,19 +3447,19 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="K17" t="s" s="2">
+        <v>175</v>
+      </c>
+      <c r="L17" t="s" s="2">
         <v>176</v>
       </c>
-      <c r="K17" t="s" s="2">
+      <c r="M17" t="s" s="2">
         <v>177</v>
       </c>
-      <c r="L17" t="s" s="2">
+      <c r="N17" t="s" s="2">
         <v>178</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>179</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>180</v>
       </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
@@ -3447,13 +3484,11 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X17" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>155</v>
+      </c>
+      <c r="X17" s="2"/>
       <c r="Y17" t="s" s="2">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3471,10 +3506,10 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>55</v>
@@ -3486,10 +3521,10 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
+        <v>180</v>
+      </c>
+      <c r="AK17" t="s" s="2">
         <v>181</v>
-      </c>
-      <c r="AK17" t="s" s="2">
-        <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>182</v>
@@ -3501,12 +3536,12 @@
         <v>184</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>45</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3514,10 +3549,10 @@
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>45</v>
@@ -3529,18 +3564,20 @@
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>189</v>
-      </c>
-      <c r="N18" s="2"/>
+        <v>190</v>
+      </c>
+      <c r="N18" t="s" s="2">
+        <v>191</v>
+      </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
       </c>
@@ -3588,13 +3625,13 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>45</v>
@@ -3603,19 +3640,19 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>45</v>
+        <v>192</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>184</v>
+        <v>195</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3623,18 +3660,18 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>45</v>
@@ -3646,20 +3683,18 @@
         <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="N19" t="s" s="2">
-        <v>197</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
         <v>45</v>
       </c>
@@ -3707,13 +3742,13 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>45</v>
@@ -3722,19 +3757,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>198</v>
+        <v>45</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3865,7 +3900,7 @@
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>45</v>
+        <v>214</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
@@ -3884,18 +3919,20 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="N21" s="2"/>
+        <v>218</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>219</v>
+      </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
       </c>
@@ -3958,19 +3995,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>45</v>
+        <v>220</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -3978,7 +4015,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3986,10 +4023,10 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F22" t="s" s="2">
         <v>55</v>
-      </c>
-      <c r="F22" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>45</v>
@@ -4001,18 +4038,18 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="M22" s="2"/>
-      <c r="N22" t="s" s="2">
-        <v>225</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
         <v>45</v>
       </c>
@@ -4060,13 +4097,13 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>45</v>
@@ -4075,19 +4112,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>226</v>
+        <v>45</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4095,7 +4132,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -4103,10 +4140,10 @@
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F23" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4118,19 +4155,17 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>153</v>
+        <v>233</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>233</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" t="s" s="2">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4179,42 +4214,42 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH23" t="s" s="2">
-        <v>235</v>
+        <v>45</v>
       </c>
       <c r="AI23" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>45</v>
+        <v>237</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>236</v>
+        <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>45</v>
+        <v>240</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>239</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -4234,22 +4269,22 @@
         <v>45</v>
       </c>
       <c r="I24" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4274,13 +4309,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>245</v>
+        <v>45</v>
       </c>
       <c r="X24" t="s" s="2">
-        <v>246</v>
+        <v>45</v>
       </c>
       <c r="Y24" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4298,7 +4333,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4307,7 +4342,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4316,10 +4351,10 @@
         <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>45</v>
+        <v>247</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>98</v>
+        <v>248</v>
       </c>
       <c r="AM24" t="s" s="2">
         <v>249</v>
@@ -4328,23 +4363,23 @@
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>45</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
-        <v>251</v>
+        <v>45</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F25" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s" s="2">
         <v>45</v>
@@ -4356,7 +4391,7 @@
         <v>45</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K25" t="s" s="2">
         <v>252</v>
@@ -4393,13 +4428,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4417,16 +4452,16 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG25" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>45</v>
+        <v>259</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4435,10 +4470,10 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>259</v>
+        <v>98</v>
       </c>
       <c r="AM25" t="s" s="2">
         <v>260</v>
@@ -4447,16 +4482,16 @@
         <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>261</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>45</v>
+        <v>262</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4475,19 +4510,19 @@
         <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
+        <v>164</v>
+      </c>
+      <c r="K26" t="s" s="2">
         <v>263</v>
       </c>
-      <c r="K26" t="s" s="2">
+      <c r="L26" t="s" s="2">
         <v>264</v>
       </c>
-      <c r="L26" t="s" s="2">
+      <c r="M26" t="s" s="2">
         <v>265</v>
       </c>
-      <c r="M26" t="s" s="2">
+      <c r="N26" t="s" s="2">
         <v>266</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>267</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4512,13 +4547,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>45</v>
+        <v>268</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4536,7 +4571,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4554,24 +4589,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>45</v>
+        <v>269</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>45</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4582,7 +4617,7 @@
         <v>43</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>45</v>
@@ -4594,18 +4629,20 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>153</v>
+        <v>274</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="N27" s="2"/>
+        <v>277</v>
+      </c>
+      <c r="N27" t="s" s="2">
+        <v>278</v>
+      </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
       </c>
@@ -4629,13 +4666,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>274</v>
+        <v>45</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>275</v>
+        <v>45</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>276</v>
+        <v>45</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4653,13 +4690,13 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH27" t="s" s="2">
         <v>45</v>
@@ -4671,19 +4708,19 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>277</v>
+        <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>280</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" hidden="true">
@@ -4711,7 +4748,7 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K28" t="s" s="2">
         <v>282</v>
@@ -4722,9 +4759,7 @@
       <c r="M28" t="s" s="2">
         <v>284</v>
       </c>
-      <c r="N28" t="s" s="2">
-        <v>285</v>
-      </c>
+      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4748,7 +4783,7 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>274</v>
+        <v>285</v>
       </c>
       <c r="X28" t="s" s="2">
         <v>286</v>
@@ -4790,24 +4825,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>45</v>
+        <v>288</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>45</v>
+        <v>291</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4830,18 +4865,20 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>291</v>
+        <v>164</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>294</v>
-      </c>
-      <c r="N29" s="2"/>
+        <v>295</v>
+      </c>
+      <c r="N29" t="s" s="2">
+        <v>296</v>
+      </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4865,13 +4902,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>45</v>
+        <v>297</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>45</v>
+        <v>298</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4889,7 +4926,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4907,24 +4944,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>295</v>
+        <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>298</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4947,16 +4984,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5006,7 +5043,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5024,24 +5061,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5052,7 +5089,7 @@
         <v>43</v>
       </c>
       <c r="F31" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G31" t="s" s="2">
         <v>45</v>
@@ -5064,20 +5101,18 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>312</v>
-      </c>
-      <c r="N31" t="s" s="2">
-        <v>313</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
         <v>45</v>
       </c>
@@ -5125,42 +5160,42 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG31" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI31" t="s" s="2">
-        <v>314</v>
+        <v>67</v>
       </c>
       <c r="AJ31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>45</v>
+        <v>315</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>45</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5171,7 +5206,7 @@
         <v>43</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>45</v>
@@ -5183,16 +5218,20 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>57</v>
+        <v>320</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
+        <v>322</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>324</v>
+      </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
@@ -5240,19 +5279,19 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>45</v>
+        <v>325</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>45</v>
@@ -5261,10 +5300,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5275,18 +5314,18 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
@@ -5298,17 +5337,15 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>102</v>
+        <v>329</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>104</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="M33" s="2"/>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5357,19 +5394,19 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>45</v>
@@ -5381,7 +5418,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5392,11 +5429,11 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>326</v>
+        <v>117</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
@@ -5409,26 +5446,24 @@
         <v>45</v>
       </c>
       <c r="H34" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I34" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>45</v>
       </c>
@@ -5476,7 +5511,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5500,7 +5535,7 @@
         <v>45</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>98</v>
+        <v>332</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5511,39 +5546,43 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>45</v>
+        <v>338</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F35" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G35" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>331</v>
+        <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>333</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+        <v>340</v>
+      </c>
+      <c r="M35" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="N35" t="s" s="2">
+        <v>121</v>
+      </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5591,19 +5630,19 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG35" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH35" t="s" s="2">
-        <v>334</v>
+        <v>45</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>45</v>
@@ -5612,10 +5651,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>335</v>
+        <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>336</v>
+        <v>98</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5626,7 +5665,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5649,13 +5688,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>338</v>
+        <v>344</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5706,7 +5745,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>337</v>
+        <v>342</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5715,7 +5754,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>334</v>
+        <v>346</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5727,10 +5766,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>335</v>
+        <v>347</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>340</v>
+        <v>348</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5741,7 +5780,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5764,20 +5803,16 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>153</v>
+        <v>343</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>342</v>
+        <v>350</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>344</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>345</v>
-      </c>
+        <v>351</v>
+      </c>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>45</v>
       </c>
@@ -5801,13 +5836,13 @@
         <v>45</v>
       </c>
       <c r="W37" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X37" t="s" s="2">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="Y37" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="Z37" t="s" s="2">
         <v>45</v>
@@ -5825,7 +5860,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>341</v>
+        <v>349</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5834,7 +5869,7 @@
         <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>45</v>
+        <v>346</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>67</v>
@@ -5843,13 +5878,13 @@
         <v>45</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>348</v>
+        <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>260</v>
+        <v>352</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5860,7 +5895,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5871,7 +5906,7 @@
         <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>45</v>
@@ -5883,19 +5918,19 @@
         <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5920,13 +5955,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>274</v>
+        <v>79</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -5944,13 +5979,13 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>45</v>
@@ -5962,13 +5997,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>348</v>
+        <v>360</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>349</v>
+        <v>361</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -5979,7 +6014,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -5990,7 +6025,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -6002,17 +6037,19 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>358</v>
+        <v>164</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="M39" s="2"/>
+        <v>364</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>365</v>
+      </c>
       <c r="N39" t="s" s="2">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6037,13 +6074,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>45</v>
+        <v>367</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>45</v>
+        <v>368</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6061,13 +6098,13 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH39" t="s" s="2">
         <v>45</v>
@@ -6079,13 +6116,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>45</v>
+        <v>360</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>45</v>
+        <v>361</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>362</v>
+        <v>271</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6096,7 +6133,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6119,16 +6156,18 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>57</v>
+        <v>370</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+      <c r="N40" t="s" s="2">
+        <v>373</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6176,7 +6215,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>363</v>
+        <v>369</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6197,10 +6236,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>335</v>
+        <v>45</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>366</v>
+        <v>374</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6211,7 +6250,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6222,7 +6261,7 @@
         <v>43</v>
       </c>
       <c r="F41" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G41" t="s" s="2">
         <v>45</v>
@@ -6231,20 +6270,18 @@
         <v>45</v>
       </c>
       <c r="I41" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>368</v>
+        <v>57</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>370</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>371</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6293,13 +6330,13 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>367</v>
+        <v>375</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG41" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH41" t="s" s="2">
         <v>45</v>
@@ -6314,10 +6351,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>372</v>
+        <v>347</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6328,7 +6365,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6351,16 +6388,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6410,7 +6447,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6431,10 +6468,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>372</v>
+        <v>384</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>379</v>
+        <v>385</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6445,7 +6482,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6468,20 +6505,18 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>309</v>
+        <v>387</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="N43" t="s" s="2">
-        <v>384</v>
-      </c>
+        <v>390</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6529,7 +6564,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>380</v>
+        <v>386</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6550,10 +6585,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>386</v>
+        <v>391</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6564,7 +6599,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>387</v>
+        <v>392</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6575,7 +6610,7 @@
         <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>45</v>
@@ -6584,19 +6619,23 @@
         <v>45</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>57</v>
+        <v>320</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>318</v>
+        <v>393</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>319</v>
-      </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+        <v>394</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>395</v>
+      </c>
+      <c r="N44" t="s" s="2">
+        <v>396</v>
+      </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6644,19 +6683,19 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>320</v>
+        <v>392</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI44" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ44" t="s" s="2">
         <v>45</v>
@@ -6665,10 +6704,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>45</v>
+        <v>397</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>321</v>
+        <v>398</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6679,18 +6718,18 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>388</v>
+        <v>399</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="D45" s="2"/>
       <c r="E45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6702,17 +6741,15 @@
         <v>45</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>102</v>
+        <v>329</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="M45" t="s" s="2">
-        <v>104</v>
-      </c>
+        <v>330</v>
+      </c>
+      <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -6761,19 +6798,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>106</v>
+        <v>45</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6785,7 +6822,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>321</v>
+        <v>332</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6796,11 +6833,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>389</v>
+        <v>400</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>326</v>
+        <v>117</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6813,26 +6850,24 @@
         <v>45</v>
       </c>
       <c r="H46" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>104</v>
-      </c>
-      <c r="N46" t="s" s="2">
-        <v>110</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
       </c>
@@ -6880,7 +6915,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6904,7 +6939,7 @@
         <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>98</v>
+        <v>332</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6915,42 +6950,42 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>390</v>
+        <v>401</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>45</v>
+        <v>338</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F47" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>391</v>
+        <v>339</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>392</v>
+        <v>340</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>393</v>
+        <v>120</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>167</v>
+        <v>121</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -6975,13 +7010,13 @@
         <v>45</v>
       </c>
       <c r="W47" t="s" s="2">
-        <v>274</v>
+        <v>45</v>
       </c>
       <c r="X47" t="s" s="2">
-        <v>394</v>
+        <v>45</v>
       </c>
       <c r="Y47" t="s" s="2">
-        <v>395</v>
+        <v>45</v>
       </c>
       <c r="Z47" t="s" s="2">
         <v>45</v>
@@ -6999,34 +7034,34 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>390</v>
+        <v>341</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG47" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>396</v>
+        <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>171</v>
+        <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>172</v>
+        <v>98</v>
       </c>
       <c r="AN47" t="s" s="2">
-        <v>173</v>
+        <v>45</v>
       </c>
       <c r="AO47" t="s" s="2">
         <v>45</v>
@@ -7034,7 +7069,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7042,7 +7077,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F48" t="s" s="2">
         <v>55</v>
@@ -7057,19 +7092,19 @@
         <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>398</v>
+        <v>164</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>232</v>
+        <v>404</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>234</v>
+        <v>178</v>
       </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
@@ -7094,13 +7129,13 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>45</v>
+        <v>285</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>45</v>
+        <v>406</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>45</v>
+        <v>407</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7118,10 +7153,10 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>55</v>
@@ -7136,24 +7171,24 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>238</v>
+        <v>183</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>45</v>
+        <v>184</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>239</v>
+        <v>45</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7173,22 +7208,22 @@
         <v>45</v>
       </c>
       <c r="I49" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>153</v>
+        <v>410</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>403</v>
+        <v>411</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>404</v>
+        <v>243</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7213,13 +7248,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>245</v>
+        <v>45</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>246</v>
+        <v>45</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7237,7 +7272,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7246,7 +7281,7 @@
         <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="AI49" t="s" s="2">
         <v>67</v>
@@ -7255,10 +7290,10 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>45</v>
+        <v>413</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>98</v>
+        <v>248</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>249</v>
@@ -7267,23 +7302,23 @@
         <v>45</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>45</v>
+        <v>250</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>251</v>
+        <v>45</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>45</v>
@@ -7295,16 +7330,16 @@
         <v>45</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>153</v>
+        <v>164</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>252</v>
+        <v>415</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>253</v>
+        <v>416</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>254</v>
+        <v>417</v>
       </c>
       <c r="N50" t="s" s="2">
         <v>255</v>
@@ -7332,13 +7367,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>245</v>
+        <v>256</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7356,16 +7391,16 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>406</v>
+        <v>414</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>45</v>
+        <v>259</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>67</v>
@@ -7374,10 +7409,10 @@
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>259</v>
+        <v>98</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>260</v>
@@ -7386,16 +7421,16 @@
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>261</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>45</v>
+        <v>262</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -7414,19 +7449,19 @@
         <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>408</v>
+        <v>263</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>409</v>
+        <v>264</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>312</v>
+        <v>265</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>313</v>
+        <v>266</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7451,13 +7486,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>45</v>
+        <v>256</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>45</v>
+        <v>268</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7475,7 +7510,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>407</v>
+        <v>418</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7493,23 +7528,142 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>45</v>
+        <v>269</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>315</v>
+        <v>270</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>316</v>
+        <v>271</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="52" hidden="true">
+      <c r="A52" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D52" s="2"/>
+      <c r="E52" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K52" t="s" s="2">
+        <v>420</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>421</v>
+      </c>
+      <c r="M52" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="N52" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="O52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P52" s="2"/>
+      <c r="Q52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE52" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="AF52" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG52" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI52" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL52" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="AM52" t="s" s="2">
+        <v>327</v>
+      </c>
+      <c r="AN52" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO52" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO51">
+  <autoFilter ref="A1:AO52">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7519,7 +7673,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI50">
+  <conditionalFormatting sqref="A2:AI51">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added prior level of function
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-fs.xlsx
+++ b/build/output/StructureDefinition-pacio-fs.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$55</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="430">
   <si>
     <t>Path</t>
   </si>
@@ -379,6 +379,33 @@
   </si>
   <si>
     <t>.participation[typeCode=LOC].role</t>
+  </si>
+  <si>
+    <t>grouped-functionalStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://paciowg.github.io/functional-status-ig/StructureDefinition/grouped-functionalStatus}
+</t>
+  </si>
+  <si>
+    <t>Optional Extensions Element</t>
+  </si>
+  <si>
+    <t>Optional Extension Element - found in all resources.</t>
+  </si>
+  <si>
+    <t>grouping-order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://paciowg.github.io/functional-status-ig/StructureDefinition/grouping-order}
+</t>
+  </si>
+  <si>
+    <t>grouping-name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://paciowg.github.io/functional-status-ig/StructureDefinition/grouping-name}
+</t>
   </si>
   <si>
     <t>Observation.modifierExtension</t>
@@ -1488,7 +1515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO52"/>
+  <dimension ref="A1:AO55"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1498,7 +1525,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.9921875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="23.8203125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -2716,11 +2743,13 @@
     </row>
     <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s" s="2">
         <v>116</v>
       </c>
-      <c r="B11" s="2"/>
       <c r="C11" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" t="s" s="2">
@@ -2733,13 +2762,13 @@
         <v>45</v>
       </c>
       <c r="H11" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I11" t="s" s="2">
         <v>45</v>
       </c>
       <c r="J11" t="s" s="2">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="K11" t="s" s="2">
         <v>118</v>
@@ -2747,12 +2776,8 @@
       <c r="L11" t="s" s="2">
         <v>119</v>
       </c>
-      <c r="M11" t="s" s="2">
-        <v>120</v>
-      </c>
-      <c r="N11" t="s" s="2">
-        <v>121</v>
-      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
       <c r="O11" t="s" s="2">
         <v>45</v>
       </c>
@@ -2800,7 +2825,7 @@
         <v>45</v>
       </c>
       <c r="AE11" t="s" s="2">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="AF11" t="s" s="2">
         <v>43</v>
@@ -2809,7 +2834,7 @@
         <v>44</v>
       </c>
       <c r="AH11" t="s" s="2">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="AI11" t="s" s="2">
         <v>106</v>
@@ -2835,9 +2860,11 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="B12" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="B12" t="s" s="2">
+        <v>120</v>
+      </c>
       <c r="C12" t="s" s="2">
         <v>45</v>
       </c>
@@ -2846,7 +2873,7 @@
         <v>43</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>45</v>
@@ -2855,21 +2882,19 @@
         <v>45</v>
       </c>
       <c r="I12" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="M12" s="2"/>
-      <c r="N12" t="s" s="2">
-        <v>127</v>
-      </c>
+      <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
         <v>45</v>
       </c>
@@ -2917,7 +2942,7 @@
         <v>45</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>43</v>
@@ -2926,25 +2951,25 @@
         <v>44</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ12" t="s" s="2">
-        <v>128</v>
+        <v>45</v>
       </c>
       <c r="AK12" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>129</v>
+        <v>45</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>131</v>
+        <v>45</v>
       </c>
       <c r="AO12" t="s" s="2">
         <v>45</v>
@@ -2952,18 +2977,20 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>132</v>
-      </c>
-      <c r="B13" s="2"/>
+        <v>99</v>
+      </c>
+      <c r="B13" t="s" s="2">
+        <v>122</v>
+      </c>
       <c r="C13" t="s" s="2">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>45</v>
@@ -2972,21 +2999,19 @@
         <v>45</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="N13" t="s" s="2">
-        <v>137</v>
-      </c>
+      <c r="N13" s="2"/>
       <c r="O13" t="s" s="2">
         <v>45</v>
       </c>
@@ -3034,7 +3059,7 @@
         <v>45</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>132</v>
+        <v>105</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>43</v>
@@ -3043,22 +3068,22 @@
         <v>44</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>45</v>
+        <v>112</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="AN13" t="s" s="2">
         <v>45</v>
@@ -3069,11 +3094,11 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -3086,24 +3111,26 @@
         <v>45</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J14" t="s" s="2">
-        <v>143</v>
+        <v>100</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>144</v>
+        <v>126</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>145</v>
+        <v>127</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>146</v>
-      </c>
-      <c r="N14" s="2"/>
+        <v>128</v>
+      </c>
+      <c r="N14" t="s" s="2">
+        <v>129</v>
+      </c>
       <c r="O14" t="s" s="2">
         <v>45</v>
       </c>
@@ -3151,7 +3178,7 @@
         <v>45</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>43</v>
@@ -3163,19 +3190,19 @@
         <v>45</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>147</v>
+        <v>45</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>148</v>
+        <v>45</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>149</v>
+        <v>98</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>45</v>
@@ -3186,7 +3213,7 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
@@ -3194,34 +3221,32 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H15" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I15" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>151</v>
+        <v>133</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>152</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>153</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="M15" s="2"/>
       <c r="N15" t="s" s="2">
-        <v>154</v>
+        <v>135</v>
       </c>
       <c r="O15" t="s" s="2">
         <v>45</v>
@@ -3246,13 +3271,13 @@
         <v>45</v>
       </c>
       <c r="W15" t="s" s="2">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>157</v>
+        <v>45</v>
       </c>
       <c r="Z15" t="s" s="2">
         <v>45</v>
@@ -3270,13 +3295,13 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>45</v>
@@ -3285,19 +3310,19 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>159</v>
+        <v>45</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3305,11 +3330,11 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
@@ -3325,22 +3350,20 @@
         <v>45</v>
       </c>
       <c r="I16" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>167</v>
-      </c>
+        <v>144</v>
+      </c>
+      <c r="M16" s="2"/>
       <c r="N16" t="s" s="2">
-        <v>168</v>
+        <v>145</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3365,13 +3388,13 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>170</v>
+        <v>45</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3389,7 +3412,7 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>43</v>
@@ -3404,19 +3427,19 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>45</v>
+        <v>147</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3424,18 +3447,18 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F17" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G17" t="s" s="2">
         <v>45</v>
@@ -3447,20 +3470,18 @@
         <v>56</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>175</v>
+        <v>152</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>176</v>
+        <v>153</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>178</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
         <v>45</v>
       </c>
@@ -3484,11 +3505,13 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="X17" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="X17" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="Y17" t="s" s="2">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3506,13 +3529,13 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>45</v>
@@ -3521,27 +3544,27 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>184</v>
+        <v>45</v>
       </c>
       <c r="AO17" t="s" s="2">
-        <v>185</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
@@ -3558,25 +3581,25 @@
         <v>45</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I18" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>187</v>
+        <v>75</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>188</v>
+        <v>159</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>190</v>
+        <v>161</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>191</v>
+        <v>162</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3601,13 +3624,13 @@
         <v>45</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="X18" t="s" s="2">
-        <v>45</v>
+        <v>164</v>
       </c>
       <c r="Y18" t="s" s="2">
-        <v>45</v>
+        <v>165</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>45</v>
@@ -3625,10 +3648,10 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>55</v>
@@ -3640,19 +3663,19 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>45</v>
+        <v>167</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>193</v>
+        <v>168</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>194</v>
+        <v>169</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>195</v>
+        <v>170</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>45</v>
@@ -3660,7 +3683,7 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3680,21 +3703,23 @@
         <v>45</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>197</v>
+        <v>172</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>198</v>
+        <v>173</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>200</v>
-      </c>
-      <c r="N19" s="2"/>
+        <v>175</v>
+      </c>
+      <c r="N19" t="s" s="2">
+        <v>176</v>
+      </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
       </c>
@@ -3718,13 +3743,13 @@
         <v>45</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>45</v>
+        <v>177</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>45</v>
@@ -3742,7 +3767,7 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>196</v>
+        <v>171</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
@@ -3763,13 +3788,13 @@
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>195</v>
+        <v>180</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3777,15 +3802,15 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>203</v>
+        <v>182</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F20" t="s" s="2">
         <v>55</v>
@@ -3800,19 +3825,19 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="O20" t="s" s="2">
         <v>45</v>
@@ -3837,13 +3862,11 @@
         <v>45</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X20" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="X20" s="2"/>
       <c r="Y20" t="s" s="2">
-        <v>45</v>
+        <v>187</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>45</v>
@@ -3861,10 +3884,10 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>55</v>
@@ -3876,35 +3899,35 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>211</v>
+        <v>191</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>212</v>
+        <v>192</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>45</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>214</v>
+        <v>45</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>55</v>
@@ -3919,19 +3942,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>218</v>
+        <v>198</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -3980,7 +4003,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>213</v>
+        <v>194</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -3995,19 +4018,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>222</v>
+        <v>202</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4015,7 +4038,7 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -4026,7 +4049,7 @@
         <v>43</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>45</v>
@@ -4038,16 +4061,16 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>228</v>
+        <v>208</v>
       </c>
       <c r="N22" s="2"/>
       <c r="O22" t="s" s="2">
@@ -4097,13 +4120,13 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>224</v>
+        <v>204</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>45</v>
@@ -4118,13 +4141,13 @@
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>229</v>
+        <v>190</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>231</v>
+        <v>203</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4132,18 +4155,18 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>45</v>
+        <v>211</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F23" t="s" s="2">
         <v>55</v>
-      </c>
-      <c r="F23" t="s" s="2">
-        <v>44</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>45</v>
@@ -4155,17 +4178,19 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>214</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>215</v>
+      </c>
       <c r="N23" t="s" s="2">
-        <v>236</v>
+        <v>216</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>45</v>
@@ -4214,13 +4239,13 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>232</v>
+        <v>210</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG23" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH23" t="s" s="2">
         <v>45</v>
@@ -4229,19 +4254,19 @@
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>239</v>
+        <v>219</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4249,11 +4274,11 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>45</v>
+        <v>222</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
@@ -4272,19 +4297,19 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>164</v>
+        <v>223</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>242</v>
+        <v>224</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>243</v>
+        <v>225</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>244</v>
+        <v>226</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>245</v>
+        <v>227</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4309,11 +4334,13 @@
         <v>45</v>
       </c>
       <c r="W24" t="s" s="2">
-        <v>155</v>
-      </c>
-      <c r="X24" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="X24" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="Y24" t="s" s="2">
-        <v>179</v>
+        <v>45</v>
       </c>
       <c r="Z24" t="s" s="2">
         <v>45</v>
@@ -4331,7 +4358,7 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
@@ -4340,33 +4367,33 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>246</v>
+        <v>45</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>45</v>
+        <v>228</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>247</v>
+        <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>248</v>
+        <v>229</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>249</v>
+        <v>230</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>45</v>
+        <v>231</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4386,23 +4413,21 @@
         <v>45</v>
       </c>
       <c r="I25" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>164</v>
+        <v>233</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>252</v>
+        <v>234</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>255</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4426,13 +4451,13 @@
         <v>45</v>
       </c>
       <c r="W25" t="s" s="2">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>257</v>
+        <v>45</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4450,7 +4475,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>251</v>
+        <v>232</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4459,7 +4484,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>259</v>
+        <v>45</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4471,13 +4496,13 @@
         <v>45</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>45</v>
+        <v>239</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>45</v>
@@ -4485,15 +4510,15 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>262</v>
+        <v>45</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>44</v>
@@ -4505,22 +4530,20 @@
         <v>45</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>164</v>
+        <v>241</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>263</v>
+        <v>242</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="M26" t="s" s="2">
-        <v>265</v>
-      </c>
+        <v>243</v>
+      </c>
+      <c r="M26" s="2"/>
       <c r="N26" t="s" s="2">
-        <v>266</v>
+        <v>244</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4545,13 +4568,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>268</v>
+        <v>45</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4569,7 +4592,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4584,27 +4607,27 @@
         <v>67</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>45</v>
+        <v>245</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>269</v>
+        <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>271</v>
+        <v>247</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>272</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4615,7 +4638,7 @@
         <v>43</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>45</v>
@@ -4624,22 +4647,22 @@
         <v>45</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>274</v>
+        <v>172</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4664,13 +4687,11 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X27" t="s" s="2">
-        <v>45</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="X27" s="2"/>
       <c r="Y27" t="s" s="2">
-        <v>45</v>
+        <v>187</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4688,16 +4709,16 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>273</v>
+        <v>249</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>45</v>
+        <v>254</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>67</v>
@@ -4706,24 +4727,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>45</v>
+        <v>255</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>279</v>
+        <v>256</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>280</v>
+        <v>257</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>45</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4746,18 +4767,20 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>282</v>
+        <v>260</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>284</v>
-      </c>
-      <c r="N28" s="2"/>
+        <v>262</v>
+      </c>
+      <c r="N28" t="s" s="2">
+        <v>263</v>
+      </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
       </c>
@@ -4781,13 +4804,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>286</v>
+        <v>265</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>287</v>
+        <v>266</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4805,7 +4828,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>281</v>
+        <v>259</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4814,7 +4837,7 @@
         <v>55</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>67</v>
@@ -4823,35 +4846,35 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>288</v>
+        <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>289</v>
+        <v>98</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>290</v>
+        <v>268</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>291</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>45</v>
+        <v>270</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>45</v>
@@ -4863,19 +4886,19 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>294</v>
+        <v>272</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>295</v>
+        <v>273</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>296</v>
+        <v>274</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
@@ -4900,13 +4923,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>285</v>
+        <v>264</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>297</v>
+        <v>275</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>298</v>
+        <v>276</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4924,13 +4947,13 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>292</v>
+        <v>269</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>45</v>
@@ -4942,24 +4965,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>45</v>
+        <v>277</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>299</v>
+        <v>278</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>45</v>
+        <v>280</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4970,7 +4993,7 @@
         <v>43</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>45</v>
@@ -4982,18 +5005,20 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>304</v>
+        <v>284</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>305</v>
-      </c>
-      <c r="N30" s="2"/>
+        <v>285</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>286</v>
+      </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
       </c>
@@ -5041,13 +5066,13 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>45</v>
@@ -5059,24 +5084,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>306</v>
+        <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>307</v>
+        <v>287</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>308</v>
+        <v>288</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>309</v>
+        <v>45</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5099,16 +5124,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>311</v>
+        <v>172</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>312</v>
+        <v>290</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>313</v>
+        <v>291</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>314</v>
+        <v>292</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5134,13 +5159,13 @@
         <v>45</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>45</v>
+        <v>294</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>45</v>
+        <v>295</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>45</v>
@@ -5158,7 +5183,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>289</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5176,24 +5201,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>315</v>
+        <v>296</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>316</v>
+        <v>297</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>317</v>
+        <v>298</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>318</v>
+        <v>299</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5204,7 +5229,7 @@
         <v>43</v>
       </c>
       <c r="F32" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s" s="2">
         <v>45</v>
@@ -5216,19 +5241,19 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>320</v>
+        <v>172</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>321</v>
+        <v>301</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>322</v>
+        <v>302</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>323</v>
+        <v>303</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>324</v>
+        <v>304</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
@@ -5253,13 +5278,13 @@
         <v>45</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>45</v>
+        <v>305</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>45</v>
+        <v>306</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>45</v>
@@ -5277,19 +5302,19 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>319</v>
+        <v>300</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG32" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>325</v>
+        <v>67</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>45</v>
@@ -5298,10 +5323,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>326</v>
+        <v>307</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>327</v>
+        <v>308</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5312,7 +5337,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5335,15 +5360,17 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>57</v>
+        <v>310</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M33" s="2"/>
+        <v>312</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>313</v>
+      </c>
       <c r="N33" s="2"/>
       <c r="O33" t="s" s="2">
         <v>45</v>
@@ -5392,7 +5419,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>331</v>
+        <v>309</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5404,41 +5431,41 @@
         <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>45</v>
+        <v>314</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>45</v>
+        <v>315</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>45</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2"/>
       <c r="E34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F34" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G34" t="s" s="2">
         <v>45</v>
@@ -5450,16 +5477,16 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>100</v>
+        <v>319</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>120</v>
+        <v>322</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
@@ -5509,46 +5536,46 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>336</v>
+        <v>318</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG34" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>45</v>
+        <v>323</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>45</v>
+        <v>324</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>45</v>
+        <v>326</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>338</v>
+        <v>45</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5561,25 +5588,25 @@
         <v>45</v>
       </c>
       <c r="H35" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I35" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>100</v>
+        <v>328</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>120</v>
+        <v>331</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>121</v>
+        <v>332</v>
       </c>
       <c r="O35" t="s" s="2">
         <v>45</v>
@@ -5628,7 +5655,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5640,7 +5667,7 @@
         <v>45</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>106</v>
+        <v>333</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>45</v>
@@ -5649,10 +5676,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>45</v>
+        <v>334</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>98</v>
+        <v>335</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5663,7 +5690,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5686,13 +5713,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>343</v>
+        <v>57</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5743,7 +5770,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5752,10 +5779,10 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>45</v>
@@ -5764,10 +5791,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5778,18 +5805,18 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
@@ -5801,15 +5828,17 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
+        <v>100</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>342</v>
+      </c>
+      <c r="L37" t="s" s="2">
         <v>343</v>
       </c>
-      <c r="K37" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="M37" s="2"/>
+      <c r="M37" t="s" s="2">
+        <v>128</v>
+      </c>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5858,19 +5887,19 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>45</v>
@@ -5879,10 +5908,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>347</v>
+        <v>45</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>352</v>
+        <v>340</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5893,42 +5922,42 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>45</v>
+        <v>346</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>356</v>
+        <v>128</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>357</v>
+        <v>129</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5953,13 +5982,13 @@
         <v>45</v>
       </c>
       <c r="W38" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>358</v>
+        <v>45</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>359</v>
+        <v>45</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -5977,31 +6006,31 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH38" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>360</v>
+        <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>361</v>
+        <v>45</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>271</v>
+        <v>98</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6012,7 +6041,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6023,7 +6052,7 @@
         <v>43</v>
       </c>
       <c r="F39" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G39" t="s" s="2">
         <v>45</v>
@@ -6035,20 +6064,16 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>164</v>
+        <v>351</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>364</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>365</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>366</v>
-      </c>
+        <v>353</v>
+      </c>
+      <c r="M39" s="2"/>
+      <c r="N39" s="2"/>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6072,13 +6097,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>367</v>
+        <v>45</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>368</v>
+        <v>45</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6096,16 +6121,16 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>362</v>
+        <v>350</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG39" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>45</v>
+        <v>354</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>67</v>
@@ -6114,13 +6139,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>360</v>
+        <v>45</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>271</v>
+        <v>356</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6131,7 +6156,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6154,18 +6179,16 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>370</v>
+        <v>351</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>371</v>
+        <v>358</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>372</v>
+        <v>359</v>
       </c>
       <c r="M40" s="2"/>
-      <c r="N40" t="s" s="2">
-        <v>373</v>
-      </c>
+      <c r="N40" s="2"/>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6213,7 +6236,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6222,7 +6245,7 @@
         <v>55</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>45</v>
+        <v>354</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>67</v>
@@ -6234,10 +6257,10 @@
         <v>45</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>45</v>
+        <v>355</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6248,7 +6271,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6271,16 +6294,20 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>57</v>
+        <v>172</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>376</v>
+        <v>362</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>377</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
+        <v>363</v>
+      </c>
+      <c r="M41" t="s" s="2">
+        <v>364</v>
+      </c>
+      <c r="N41" t="s" s="2">
+        <v>365</v>
+      </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
       </c>
@@ -6304,13 +6331,13 @@
         <v>45</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>45</v>
+        <v>366</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>45</v>
+        <v>367</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>45</v>
@@ -6328,7 +6355,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>375</v>
+        <v>361</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6346,13 +6373,13 @@
         <v>45</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>45</v>
+        <v>368</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>347</v>
+        <v>369</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>378</v>
+        <v>279</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6363,7 +6390,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6383,21 +6410,23 @@
         <v>45</v>
       </c>
       <c r="I42" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>380</v>
+        <v>172</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>383</v>
-      </c>
-      <c r="N42" s="2"/>
+        <v>373</v>
+      </c>
+      <c r="N42" t="s" s="2">
+        <v>374</v>
+      </c>
       <c r="O42" t="s" s="2">
         <v>45</v>
       </c>
@@ -6421,13 +6450,13 @@
         <v>45</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>45</v>
+        <v>293</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>45</v>
+        <v>375</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>45</v>
+        <v>376</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>45</v>
@@ -6445,7 +6474,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6463,13 +6492,13 @@
         <v>45</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>45</v>
+        <v>368</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>384</v>
+        <v>369</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>385</v>
+        <v>279</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6480,7 +6509,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6491,7 +6520,7 @@
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
@@ -6500,21 +6529,21 @@
         <v>45</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>389</v>
-      </c>
-      <c r="M43" t="s" s="2">
-        <v>390</v>
-      </c>
-      <c r="N43" s="2"/>
+        <v>380</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" t="s" s="2">
+        <v>381</v>
+      </c>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6562,13 +6591,13 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>45</v>
@@ -6583,10 +6612,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>384</v>
+        <v>45</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6597,7 +6626,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6608,7 +6637,7 @@
         <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>45</v>
@@ -6617,23 +6646,19 @@
         <v>45</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>320</v>
+        <v>57</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>394</v>
-      </c>
-      <c r="M44" t="s" s="2">
-        <v>395</v>
-      </c>
-      <c r="N44" t="s" s="2">
-        <v>396</v>
-      </c>
+        <v>385</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
       </c>
@@ -6681,13 +6706,13 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>45</v>
@@ -6702,10 +6727,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>397</v>
+        <v>355</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>398</v>
+        <v>386</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6716,7 +6741,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6727,7 +6752,7 @@
         <v>43</v>
       </c>
       <c r="F45" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G45" t="s" s="2">
         <v>45</v>
@@ -6736,18 +6761,20 @@
         <v>45</v>
       </c>
       <c r="I45" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>57</v>
+        <v>388</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>329</v>
+        <v>389</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>330</v>
-      </c>
-      <c r="M45" s="2"/>
+        <v>390</v>
+      </c>
+      <c r="M45" t="s" s="2">
+        <v>391</v>
+      </c>
       <c r="N45" s="2"/>
       <c r="O45" t="s" s="2">
         <v>45</v>
@@ -6796,19 +6823,19 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>331</v>
+        <v>387</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG45" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH45" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI45" t="s" s="2">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="AJ45" t="s" s="2">
         <v>45</v>
@@ -6817,10 +6844,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>45</v>
+        <v>392</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>332</v>
+        <v>393</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6831,11 +6858,11 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" t="s" s="2">
@@ -6851,19 +6878,19 @@
         <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>100</v>
+        <v>395</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>334</v>
+        <v>396</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>335</v>
+        <v>397</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>120</v>
+        <v>398</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
@@ -6913,7 +6940,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>336</v>
+        <v>394</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6925,7 +6952,7 @@
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6934,10 +6961,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>45</v>
+        <v>392</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>332</v>
+        <v>399</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6948,11 +6975,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>338</v>
+        <v>45</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6965,25 +6992,25 @@
         <v>45</v>
       </c>
       <c r="H47" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I47" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>100</v>
+        <v>328</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>339</v>
+        <v>401</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>340</v>
+        <v>402</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>120</v>
+        <v>403</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>121</v>
+        <v>404</v>
       </c>
       <c r="O47" t="s" s="2">
         <v>45</v>
@@ -7032,7 +7059,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>341</v>
+        <v>400</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7044,7 +7071,7 @@
         <v>45</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>45</v>
@@ -7053,10 +7080,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>45</v>
+        <v>405</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>98</v>
+        <v>406</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7067,7 +7094,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>402</v>
+        <v>407</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7075,7 +7102,7 @@
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
         <v>55</v>
@@ -7087,23 +7114,19 @@
         <v>45</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>164</v>
+        <v>57</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>403</v>
+        <v>337</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>404</v>
-      </c>
-      <c r="M48" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="N48" t="s" s="2">
-        <v>178</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
       <c r="O48" t="s" s="2">
         <v>45</v>
       </c>
@@ -7127,13 +7150,13 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>285</v>
+        <v>45</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>406</v>
+        <v>45</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>407</v>
+        <v>45</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7151,10 +7174,10 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>402</v>
+        <v>339</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>55</v>
@@ -7163,22 +7186,22 @@
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>408</v>
+        <v>45</v>
       </c>
       <c r="AL48" t="s" s="2">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>183</v>
+        <v>340</v>
       </c>
       <c r="AN48" t="s" s="2">
-        <v>184</v>
+        <v>45</v>
       </c>
       <c r="AO48" t="s" s="2">
         <v>45</v>
@@ -7186,18 +7209,18 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
@@ -7206,23 +7229,21 @@
         <v>45</v>
       </c>
       <c r="I49" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>410</v>
+        <v>100</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>411</v>
+        <v>342</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>243</v>
+        <v>343</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>412</v>
-      </c>
-      <c r="N49" t="s" s="2">
-        <v>245</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="N49" s="2"/>
       <c r="O49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7270,77 +7291,77 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>409</v>
+        <v>344</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>413</v>
+        <v>45</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>249</v>
+        <v>340</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>250</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>45</v>
+        <v>346</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I50" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>164</v>
+        <v>100</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>415</v>
+        <v>347</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>416</v>
+        <v>348</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>417</v>
+        <v>128</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>255</v>
+        <v>129</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7365,13 +7386,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>256</v>
+        <v>45</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>257</v>
+        <v>45</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>258</v>
+        <v>45</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7389,19 +7410,19 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>414</v>
+        <v>349</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>259</v>
+        <v>45</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>45</v>
@@ -7410,10 +7431,10 @@
         <v>45</v>
       </c>
       <c r="AL50" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AM50" t="s" s="2">
         <v>98</v>
-      </c>
-      <c r="AM50" t="s" s="2">
-        <v>260</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
@@ -7424,18 +7445,18 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>262</v>
+        <v>45</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G51" t="s" s="2">
         <v>45</v>
@@ -7444,22 +7465,22 @@
         <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>263</v>
+        <v>411</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>264</v>
+        <v>412</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>265</v>
+        <v>413</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>266</v>
+        <v>186</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7484,13 +7505,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>256</v>
+        <v>293</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>267</v>
+        <v>414</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>268</v>
+        <v>415</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7508,13 +7529,13 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG51" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
         <v>45</v>
@@ -7526,24 +7547,24 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>269</v>
+        <v>416</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>270</v>
+        <v>190</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>271</v>
+        <v>191</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>45</v>
+        <v>192</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>272</v>
+        <v>45</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7554,7 +7575,7 @@
         <v>43</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>45</v>
@@ -7563,22 +7584,22 @@
         <v>45</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>45</v>
+        <v>418</v>
       </c>
       <c r="K52" t="s" s="2">
+        <v>419</v>
+      </c>
+      <c r="L52" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="M52" t="s" s="2">
         <v>420</v>
       </c>
-      <c r="L52" t="s" s="2">
-        <v>421</v>
-      </c>
-      <c r="M52" t="s" s="2">
-        <v>323</v>
-      </c>
       <c r="N52" t="s" s="2">
-        <v>324</v>
+        <v>253</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7627,13 +7648,13 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>45</v>
@@ -7645,23 +7666,380 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>45</v>
+        <v>421</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>326</v>
+        <v>256</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>327</v>
+        <v>257</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="53" hidden="true">
+      <c r="A53" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="B53" s="2"/>
+      <c r="C53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D53" s="2"/>
+      <c r="E53" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F53" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="G53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J53" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="K53" t="s" s="2">
+        <v>423</v>
+      </c>
+      <c r="L53" t="s" s="2">
+        <v>424</v>
+      </c>
+      <c r="M53" t="s" s="2">
+        <v>425</v>
+      </c>
+      <c r="N53" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="O53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P53" s="2"/>
+      <c r="Q53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W53" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="X53" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="Y53" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="Z53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE53" t="s" s="2">
+        <v>422</v>
+      </c>
+      <c r="AF53" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG53" t="s" s="2">
+        <v>55</v>
+      </c>
+      <c r="AH53" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="AI53" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL53" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="AM53" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="AN53" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO53" t="s" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" hidden="true">
+      <c r="A54" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="B54" s="2"/>
+      <c r="C54" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="D54" s="2"/>
+      <c r="E54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J54" t="s" s="2">
+        <v>172</v>
+      </c>
+      <c r="K54" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="L54" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="M54" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="N54" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="O54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P54" s="2"/>
+      <c r="Q54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W54" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="X54" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="Y54" t="s" s="2">
+        <v>276</v>
+      </c>
+      <c r="Z54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE54" t="s" s="2">
+        <v>426</v>
+      </c>
+      <c r="AF54" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG54" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI54" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK54" t="s" s="2">
+        <v>277</v>
+      </c>
+      <c r="AL54" t="s" s="2">
+        <v>278</v>
+      </c>
+      <c r="AM54" t="s" s="2">
+        <v>279</v>
+      </c>
+      <c r="AN54" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO54" t="s" s="2">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="55" hidden="true">
+      <c r="A55" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="D55" s="2"/>
+      <c r="E55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="G55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="H55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="J55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="K55" t="s" s="2">
+        <v>428</v>
+      </c>
+      <c r="L55" t="s" s="2">
+        <v>429</v>
+      </c>
+      <c r="M55" t="s" s="2">
+        <v>331</v>
+      </c>
+      <c r="N55" t="s" s="2">
+        <v>332</v>
+      </c>
+      <c r="O55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="P55" s="2"/>
+      <c r="Q55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="R55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="S55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="T55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="U55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="V55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="W55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="X55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Y55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="Z55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AA55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AB55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AC55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AD55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AE55" t="s" s="2">
+        <v>427</v>
+      </c>
+      <c r="AF55" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="AG55" t="s" s="2">
+        <v>44</v>
+      </c>
+      <c r="AH55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AI55" t="s" s="2">
+        <v>67</v>
+      </c>
+      <c r="AJ55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AK55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AL55" t="s" s="2">
+        <v>334</v>
+      </c>
+      <c r="AM55" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="AN55" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="AO55" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO52">
+  <autoFilter ref="A1:AO55">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -7671,7 +8049,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI51">
+  <conditionalFormatting sqref="A2:AI54">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Utilitze component for functional status
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-fs.xlsx
+++ b/build/output/StructureDefinition-pacio-fs.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$55</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AO$53</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="427">
   <si>
     <t>Path</t>
   </si>
@@ -381,10 +381,10 @@
     <t>.participation[typeCode=LOC].role</t>
   </si>
   <si>
-    <t>grouped-functionalStatus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://paciowg.github.io/functional-status-ig/StructureDefinition/grouped-functionalStatus}
+    <t>device-use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {https://paciowg.github.io/functional-status-ig/StructureDefinition/device-patient-used}
 </t>
   </si>
   <si>
@@ -392,20 +392,6 @@
   </si>
   <si>
     <t>Optional Extension Element - found in all resources.</t>
-  </si>
-  <si>
-    <t>grouping-order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://paciowg.github.io/functional-status-ig/StructureDefinition/grouping-order}
-</t>
-  </si>
-  <si>
-    <t>grouping-name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {https://paciowg.github.io/functional-status-ig/StructureDefinition/grouping-name}
-</t>
   </si>
   <si>
     <t>Observation.modifierExtension</t>
@@ -801,6 +787,10 @@
   </si>
   <si>
     <t>Observation.value[x]</t>
+  </si>
+  <si>
+    <t>Quantity
+CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
   </si>
   <si>
     <t>Actual result</t>
@@ -1318,7 +1308,7 @@
     <t>*All* code-value and  component.code-component.value pairs need to be taken into account to correctly understand the meaning of the observation.</t>
   </si>
   <si>
-    <t>Codes identifying names of simple observations.</t>
+    <t>The LOINC code or text of the column header (if grouped with another question).</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
@@ -1331,14 +1321,13 @@
     <t>Observation.component.value[x]</t>
   </si>
   <si>
-    <t>Quantity
-CodeableConceptstringbooleanintegerRangeRatioSampledDatatimedateTimePeriod</t>
-  </si>
-  <si>
     <t>Actual component result</t>
   </si>
   <si>
     <t>Used when observation has a set of component observations. An observation may have both a value (e.g. an  Apgar score)  and component observations (the observations from which the Apgar score was derived). If a value is present, the datatype for this element should be determined by Observation.code. A CodeableConcept with just a text would be used instead of a string if the field was usually coded, or if the type associated with the Observation.code defines a coded value.  For additional guidance, see the [Notes section](http://hl7.org/fhir/R4/observation.html#notes) below.</t>
+  </si>
+  <si>
+    <t>test desc</t>
   </si>
   <si>
     <t>363714003 |Interprets| &lt; 441742003 |Evaluation finding|</t>
@@ -1515,7 +1504,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AO55"/>
+  <dimension ref="A1:AO53"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1525,7 +1514,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="43.6015625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="23.8203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.9921875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.81640625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="5.8984375" customWidth="true" bestFit="true" hidden="true"/>
     <col min="5" max="5" width="4.69921875" customWidth="true" bestFit="true"/>
@@ -1547,7 +1536,7 @@
     <col min="21" max="21" width="16.0859375" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.078125" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.30859375" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="60.515625" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="73.45703125" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="50.89453125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.69140625" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="19.73046875" customWidth="true" bestFit="true"/>
@@ -2741,7 +2730,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" hidden="true">
+    <row r="11">
       <c r="A11" t="s" s="2">
         <v>99</v>
       </c>
@@ -2759,7 +2748,7 @@
         <v>44</v>
       </c>
       <c r="G11" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H11" t="s" s="2">
         <v>45</v>
@@ -2860,41 +2849,43 @@
     </row>
     <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B12" t="s" s="2">
         <v>120</v>
       </c>
+      <c r="B12" s="2"/>
       <c r="C12" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F12" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G12" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H12" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I12" t="s" s="2">
         <v>45</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>121</v>
+        <v>100</v>
       </c>
       <c r="K12" t="s" s="2">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="L12" t="s" s="2">
-        <v>119</v>
-      </c>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
+        <v>123</v>
+      </c>
+      <c r="M12" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="N12" t="s" s="2">
+        <v>125</v>
+      </c>
       <c r="O12" t="s" s="2">
         <v>45</v>
       </c>
@@ -2942,7 +2933,7 @@
         <v>45</v>
       </c>
       <c r="AE12" t="s" s="2">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="AF12" t="s" s="2">
         <v>43</v>
@@ -2951,7 +2942,7 @@
         <v>44</v>
       </c>
       <c r="AH12" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AI12" t="s" s="2">
         <v>106</v>
@@ -2977,11 +2968,9 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>99</v>
-      </c>
-      <c r="B13" t="s" s="2">
-        <v>122</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B13" s="2"/>
       <c r="C13" t="s" s="2">
         <v>45</v>
       </c>
@@ -2990,7 +2979,7 @@
         <v>43</v>
       </c>
       <c r="F13" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G13" t="s" s="2">
         <v>45</v>
@@ -2999,19 +2988,21 @@
         <v>45</v>
       </c>
       <c r="I13" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J13" t="s" s="2">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="N13" t="s" s="2">
+        <v>131</v>
+      </c>
       <c r="O13" t="s" s="2">
         <v>45</v>
       </c>
@@ -3059,7 +3050,7 @@
         <v>45</v>
       </c>
       <c r="AE13" t="s" s="2">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="AF13" t="s" s="2">
         <v>43</v>
@@ -3068,25 +3059,25 @@
         <v>44</v>
       </c>
       <c r="AH13" t="s" s="2">
-        <v>112</v>
+        <v>45</v>
       </c>
       <c r="AI13" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ13" t="s" s="2">
-        <v>45</v>
+        <v>132</v>
       </c>
       <c r="AK13" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL13" t="s" s="2">
-        <v>45</v>
+        <v>133</v>
       </c>
       <c r="AM13" t="s" s="2">
-        <v>98</v>
+        <v>134</v>
       </c>
       <c r="AN13" t="s" s="2">
-        <v>45</v>
+        <v>135</v>
       </c>
       <c r="AO13" t="s" s="2">
         <v>45</v>
@@ -3094,11 +3085,11 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" t="s" s="2">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
@@ -3111,25 +3102,23 @@
         <v>45</v>
       </c>
       <c r="H14" t="s" s="2">
+        <v>45</v>
+      </c>
+      <c r="I14" t="s" s="2">
         <v>56</v>
       </c>
-      <c r="I14" t="s" s="2">
-        <v>45</v>
-      </c>
       <c r="J14" t="s" s="2">
-        <v>100</v>
+        <v>138</v>
       </c>
       <c r="K14" t="s" s="2">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="L14" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="M14" t="s" s="2">
-        <v>128</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="M14" s="2"/>
       <c r="N14" t="s" s="2">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="O14" t="s" s="2">
         <v>45</v>
@@ -3178,7 +3167,7 @@
         <v>45</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="AF14" t="s" s="2">
         <v>43</v>
@@ -3190,19 +3179,19 @@
         <v>45</v>
       </c>
       <c r="AI14" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>45</v>
+        <v>142</v>
       </c>
       <c r="AK14" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL14" t="s" s="2">
-        <v>45</v>
+        <v>143</v>
       </c>
       <c r="AM14" t="s" s="2">
-        <v>98</v>
+        <v>144</v>
       </c>
       <c r="AN14" t="s" s="2">
         <v>45</v>
@@ -3213,11 +3202,11 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>45</v>
+        <v>146</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
@@ -3236,18 +3225,18 @@
         <v>56</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>134</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" t="s" s="2">
-        <v>135</v>
-      </c>
+        <v>149</v>
+      </c>
+      <c r="M15" t="s" s="2">
+        <v>150</v>
+      </c>
+      <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>45</v>
       </c>
@@ -3295,7 +3284,7 @@
         <v>45</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>131</v>
+        <v>145</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>43</v>
@@ -3310,19 +3299,19 @@
         <v>67</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL15" t="s" s="2">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="AM15" t="s" s="2">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="AN15" t="s" s="2">
-        <v>139</v>
+        <v>45</v>
       </c>
       <c r="AO15" t="s" s="2">
         <v>45</v>
@@ -3330,40 +3319,42 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>141</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G16" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H16" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I16" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>142</v>
+        <v>75</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="M16" s="2"/>
+        <v>156</v>
+      </c>
+      <c r="M16" t="s" s="2">
+        <v>157</v>
+      </c>
       <c r="N16" t="s" s="2">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="O16" t="s" s="2">
         <v>45</v>
@@ -3388,13 +3379,13 @@
         <v>45</v>
       </c>
       <c r="W16" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>45</v>
+        <v>160</v>
       </c>
       <c r="Y16" t="s" s="2">
-        <v>45</v>
+        <v>161</v>
       </c>
       <c r="Z16" t="s" s="2">
         <v>45</v>
@@ -3412,13 +3403,13 @@
         <v>45</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG16" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH16" t="s" s="2">
         <v>45</v>
@@ -3427,19 +3418,19 @@
         <v>67</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>45</v>
+        <v>163</v>
       </c>
       <c r="AL16" t="s" s="2">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="AM16" t="s" s="2">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>45</v>
+        <v>166</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>45</v>
@@ -3447,11 +3438,11 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
-        <v>150</v>
+        <v>45</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
@@ -3467,21 +3458,23 @@
         <v>45</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="N17" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="N17" t="s" s="2">
+        <v>172</v>
+      </c>
       <c r="O17" t="s" s="2">
         <v>45</v>
       </c>
@@ -3505,13 +3498,13 @@
         <v>45</v>
       </c>
       <c r="W17" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X17" t="s" s="2">
-        <v>45</v>
+        <v>173</v>
       </c>
       <c r="Y17" t="s" s="2">
-        <v>45</v>
+        <v>174</v>
       </c>
       <c r="Z17" t="s" s="2">
         <v>45</v>
@@ -3529,7 +3522,7 @@
         <v>45</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>149</v>
+        <v>167</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>43</v>
@@ -3544,19 +3537,19 @@
         <v>67</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL17" t="s" s="2">
-        <v>156</v>
+        <v>45</v>
       </c>
       <c r="AM17" t="s" s="2">
-        <v>157</v>
+        <v>175</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>45</v>
+        <v>176</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>45</v>
@@ -3564,11 +3557,11 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>45</v>
+        <v>178</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
@@ -3581,25 +3574,25 @@
         <v>45</v>
       </c>
       <c r="H18" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I18" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>75</v>
+        <v>168</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="O18" t="s" s="2">
         <v>45</v>
@@ -3624,13 +3617,11 @@
         <v>45</v>
       </c>
       <c r="W18" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="X18" t="s" s="2">
-        <v>164</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="X18" s="2"/>
       <c r="Y18" t="s" s="2">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="Z18" t="s" s="2">
         <v>45</v>
@@ -3648,7 +3639,7 @@
         <v>45</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>158</v>
+        <v>177</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>55</v>
@@ -3663,27 +3654,27 @@
         <v>67</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>166</v>
+        <v>184</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="AL18" t="s" s="2">
-        <v>168</v>
+        <v>186</v>
       </c>
       <c r="AM18" t="s" s="2">
-        <v>169</v>
+        <v>187</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>170</v>
+        <v>188</v>
       </c>
       <c r="AO18" t="s" s="2">
-        <v>45</v>
+        <v>189</v>
       </c>
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
@@ -3691,10 +3682,10 @@
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>45</v>
@@ -3703,22 +3694,22 @@
         <v>45</v>
       </c>
       <c r="I19" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>173</v>
+        <v>192</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="N19" t="s" s="2">
-        <v>176</v>
+        <v>195</v>
       </c>
       <c r="O19" t="s" s="2">
         <v>45</v>
@@ -3743,13 +3734,13 @@
         <v>45</v>
       </c>
       <c r="W19" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X19" t="s" s="2">
-        <v>177</v>
+        <v>45</v>
       </c>
       <c r="Y19" t="s" s="2">
-        <v>178</v>
+        <v>45</v>
       </c>
       <c r="Z19" t="s" s="2">
         <v>45</v>
@@ -3767,13 +3758,13 @@
         <v>45</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="AF19" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>45</v>
@@ -3782,19 +3773,19 @@
         <v>67</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>45</v>
+        <v>196</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL19" t="s" s="2">
-        <v>45</v>
+        <v>197</v>
       </c>
       <c r="AM19" t="s" s="2">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>45</v>
@@ -3802,18 +3793,18 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F20" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G20" t="s" s="2">
         <v>45</v>
@@ -3825,20 +3816,18 @@
         <v>56</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>183</v>
+        <v>202</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>185</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>186</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>45</v>
       </c>
@@ -3862,11 +3851,13 @@
         <v>45</v>
       </c>
       <c r="W20" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="X20" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="X20" t="s" s="2">
+        <v>45</v>
+      </c>
       <c r="Y20" t="s" s="2">
-        <v>187</v>
+        <v>45</v>
       </c>
       <c r="Z20" t="s" s="2">
         <v>45</v>
@@ -3884,13 +3875,13 @@
         <v>45</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG20" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH20" t="s" s="2">
         <v>45</v>
@@ -3899,35 +3890,35 @@
         <v>67</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>188</v>
+        <v>45</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>189</v>
+        <v>45</v>
       </c>
       <c r="AL20" t="s" s="2">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="AM20" t="s" s="2">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="AO20" t="s" s="2">
-        <v>193</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F21" t="s" s="2">
         <v>55</v>
@@ -3942,19 +3933,19 @@
         <v>56</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="N21" t="s" s="2">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="O21" t="s" s="2">
         <v>45</v>
@@ -4003,7 +3994,7 @@
         <v>45</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>43</v>
@@ -4018,19 +4009,19 @@
         <v>67</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>201</v>
+        <v>214</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>202</v>
+        <v>215</v>
       </c>
       <c r="AN21" t="s" s="2">
-        <v>203</v>
+        <v>216</v>
       </c>
       <c r="AO21" t="s" s="2">
         <v>45</v>
@@ -4038,18 +4029,18 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
-        <v>45</v>
+        <v>218</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F22" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G22" t="s" s="2">
         <v>45</v>
@@ -4061,18 +4052,20 @@
         <v>56</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>205</v>
+        <v>219</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>206</v>
+        <v>220</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="M22" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="N22" s="2"/>
+        <v>222</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>223</v>
+      </c>
       <c r="O22" t="s" s="2">
         <v>45</v>
       </c>
@@ -4120,13 +4113,13 @@
         <v>45</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>204</v>
+        <v>217</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG22" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH22" t="s" s="2">
         <v>45</v>
@@ -4135,19 +4128,19 @@
         <v>67</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>45</v>
+        <v>224</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="AM22" t="s" s="2">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>203</v>
+        <v>227</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>45</v>
@@ -4155,11 +4148,11 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
-        <v>211</v>
+        <v>45</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" t="s" s="2">
@@ -4178,20 +4171,18 @@
         <v>56</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="N23" t="s" s="2">
-        <v>216</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="N23" s="2"/>
       <c r="O23" t="s" s="2">
         <v>45</v>
       </c>
@@ -4239,7 +4230,7 @@
         <v>45</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>210</v>
+        <v>228</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>43</v>
@@ -4254,19 +4245,19 @@
         <v>67</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>217</v>
+        <v>45</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL23" t="s" s="2">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="AN23" t="s" s="2">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="AO23" t="s" s="2">
         <v>45</v>
@@ -4274,18 +4265,18 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
-        <v>222</v>
+        <v>45</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F24" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>45</v>
@@ -4297,19 +4288,17 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>223</v>
+        <v>237</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>224</v>
+        <v>238</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M24" t="s" s="2">
-        <v>226</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="M24" s="2"/>
       <c r="N24" t="s" s="2">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4358,13 +4347,13 @@
         <v>45</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG24" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH24" t="s" s="2">
         <v>45</v>
@@ -4373,19 +4362,19 @@
         <v>67</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="AN24" t="s" s="2">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="AO24" t="s" s="2">
         <v>45</v>
@@ -4393,7 +4382,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4416,18 +4405,20 @@
         <v>56</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="N25" s="2"/>
+        <v>249</v>
+      </c>
+      <c r="N25" t="s" s="2">
+        <v>250</v>
+      </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
       </c>
@@ -4475,7 +4466,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4484,7 +4475,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>45</v>
+        <v>251</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4493,24 +4484,24 @@
         <v>45</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>45</v>
+        <v>252</v>
       </c>
       <c r="AL25" t="s" s="2">
-        <v>237</v>
+        <v>253</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>238</v>
+        <v>254</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>239</v>
+        <v>45</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>45</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -4518,11 +4509,11 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
+        <v>43</v>
+      </c>
+      <c r="F26" t="s" s="2">
         <v>55</v>
       </c>
-      <c r="F26" t="s" s="2">
-        <v>44</v>
-      </c>
       <c r="G26" t="s" s="2">
         <v>45</v>
       </c>
@@ -4530,20 +4521,22 @@
         <v>45</v>
       </c>
       <c r="I26" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>241</v>
+        <v>168</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="M26" s="2"/>
+        <v>258</v>
+      </c>
+      <c r="M26" t="s" s="2">
+        <v>259</v>
+      </c>
       <c r="N26" t="s" s="2">
-        <v>244</v>
+        <v>260</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4568,13 +4561,13 @@
         <v>45</v>
       </c>
       <c r="W26" t="s" s="2">
-        <v>45</v>
+        <v>261</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>45</v>
+        <v>262</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>45</v>
+        <v>263</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4592,34 +4585,34 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>240</v>
+        <v>256</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG26" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH26" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="AI26" t="s" s="2">
         <v>67</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>245</v>
+        <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>246</v>
+        <v>98</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>248</v>
+        <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>45</v>
@@ -4627,18 +4620,18 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F27" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G27" t="s" s="2">
         <v>45</v>
@@ -4647,22 +4640,22 @@
         <v>45</v>
       </c>
       <c r="I27" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>250</v>
+        <v>268</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>252</v>
+        <v>270</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4687,11 +4680,13 @@
         <v>45</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>163</v>
-      </c>
-      <c r="X27" s="2"/>
+        <v>261</v>
+      </c>
+      <c r="X27" t="s" s="2">
+        <v>272</v>
+      </c>
       <c r="Y27" t="s" s="2">
-        <v>187</v>
+        <v>273</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>45</v>
@@ -4709,16 +4704,16 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG27" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH27" t="s" s="2">
-        <v>254</v>
+        <v>45</v>
       </c>
       <c r="AI27" t="s" s="2">
         <v>67</v>
@@ -4727,24 +4722,24 @@
         <v>45</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>255</v>
+        <v>274</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>258</v>
+        <v>277</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4755,7 +4750,7 @@
         <v>43</v>
       </c>
       <c r="F28" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G28" t="s" s="2">
         <v>45</v>
@@ -4767,19 +4762,19 @@
         <v>45</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>172</v>
+        <v>279</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>260</v>
+        <v>280</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>261</v>
+        <v>281</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>262</v>
+        <v>282</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>263</v>
+        <v>283</v>
       </c>
       <c r="O28" t="s" s="2">
         <v>45</v>
@@ -4804,13 +4799,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>264</v>
+        <v>45</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>266</v>
+        <v>45</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4828,16 +4823,16 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>259</v>
+        <v>278</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG28" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH28" t="s" s="2">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="AI28" t="s" s="2">
         <v>67</v>
@@ -4849,10 +4844,10 @@
         <v>45</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>98</v>
+        <v>284</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
@@ -4863,18 +4858,18 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
-        <v>270</v>
+        <v>45</v>
       </c>
       <c r="D29" s="2"/>
       <c r="E29" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F29" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G29" t="s" s="2">
         <v>45</v>
@@ -4886,20 +4881,18 @@
         <v>45</v>
       </c>
       <c r="J29" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>271</v>
+        <v>287</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>272</v>
+        <v>288</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="N29" t="s" s="2">
-        <v>274</v>
-      </c>
+        <v>289</v>
+      </c>
+      <c r="N29" s="2"/>
       <c r="O29" t="s" s="2">
         <v>45</v>
       </c>
@@ -4923,13 +4916,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>275</v>
+        <v>291</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>276</v>
+        <v>292</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4947,13 +4940,13 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG29" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH29" t="s" s="2">
         <v>45</v>
@@ -4965,24 +4958,24 @@
         <v>45</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>277</v>
+        <v>293</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>279</v>
+        <v>295</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO29" t="s" s="2">
-        <v>280</v>
+        <v>296</v>
       </c>
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4993,7 +4986,7 @@
         <v>43</v>
       </c>
       <c r="F30" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G30" t="s" s="2">
         <v>45</v>
@@ -5005,19 +4998,19 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>282</v>
+        <v>168</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="N30" t="s" s="2">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="O30" t="s" s="2">
         <v>45</v>
@@ -5042,13 +5035,13 @@
         <v>45</v>
       </c>
       <c r="W30" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="X30" t="s" s="2">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="Y30" t="s" s="2">
-        <v>45</v>
+        <v>303</v>
       </c>
       <c r="Z30" t="s" s="2">
         <v>45</v>
@@ -5066,13 +5059,13 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>281</v>
+        <v>297</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG30" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH30" t="s" s="2">
         <v>45</v>
@@ -5087,10 +5080,10 @@
         <v>45</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>287</v>
+        <v>304</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>288</v>
+        <v>305</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
@@ -5101,7 +5094,7 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5124,16 +5117,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>172</v>
+        <v>307</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5159,13 +5152,13 @@
         <v>45</v>
       </c>
       <c r="W31" t="s" s="2">
-        <v>293</v>
+        <v>45</v>
       </c>
       <c r="X31" t="s" s="2">
-        <v>294</v>
+        <v>45</v>
       </c>
       <c r="Y31" t="s" s="2">
-        <v>295</v>
+        <v>45</v>
       </c>
       <c r="Z31" t="s" s="2">
         <v>45</v>
@@ -5183,7 +5176,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>289</v>
+        <v>306</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5201,24 +5194,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>299</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5241,20 +5234,18 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>172</v>
+        <v>316</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>301</v>
+        <v>317</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>303</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>304</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="N32" s="2"/>
       <c r="O32" t="s" s="2">
         <v>45</v>
       </c>
@@ -5278,13 +5269,13 @@
         <v>45</v>
       </c>
       <c r="W32" t="s" s="2">
-        <v>293</v>
+        <v>45</v>
       </c>
       <c r="X32" t="s" s="2">
-        <v>305</v>
+        <v>45</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>306</v>
+        <v>45</v>
       </c>
       <c r="Z32" t="s" s="2">
         <v>45</v>
@@ -5302,7 +5293,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5320,24 +5311,24 @@
         <v>45</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>45</v>
+        <v>320</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>307</v>
+        <v>321</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>308</v>
+        <v>322</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO32" t="s" s="2">
-        <v>45</v>
+        <v>323</v>
       </c>
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5348,7 +5339,7 @@
         <v>43</v>
       </c>
       <c r="F33" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G33" t="s" s="2">
         <v>45</v>
@@ -5360,18 +5351,20 @@
         <v>45</v>
       </c>
       <c r="J33" t="s" s="2">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>313</v>
-      </c>
-      <c r="N33" s="2"/>
+        <v>328</v>
+      </c>
+      <c r="N33" t="s" s="2">
+        <v>329</v>
+      </c>
       <c r="O33" t="s" s="2">
         <v>45</v>
       </c>
@@ -5419,42 +5412,42 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG33" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI33" t="s" s="2">
-        <v>67</v>
+        <v>330</v>
       </c>
       <c r="AJ33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>314</v>
+        <v>45</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>315</v>
+        <v>331</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>316</v>
+        <v>332</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO33" t="s" s="2">
-        <v>317</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5477,17 +5470,15 @@
         <v>45</v>
       </c>
       <c r="J34" t="s" s="2">
-        <v>319</v>
+        <v>57</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>320</v>
+        <v>334</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>322</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="M34" s="2"/>
       <c r="N34" s="2"/>
       <c r="O34" t="s" s="2">
         <v>45</v>
@@ -5536,7 +5527,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5548,34 +5539,34 @@
         <v>45</v>
       </c>
       <c r="AI34" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>323</v>
+        <v>45</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>324</v>
+        <v>45</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>326</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>327</v>
+        <v>338</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5594,20 +5585,18 @@
         <v>45</v>
       </c>
       <c r="J35" t="s" s="2">
-        <v>328</v>
+        <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N35" t="s" s="2">
-        <v>332</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N35" s="2"/>
       <c r="O35" t="s" s="2">
         <v>45</v>
       </c>
@@ -5655,7 +5644,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>327</v>
+        <v>341</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5667,7 +5656,7 @@
         <v>45</v>
       </c>
       <c r="AI35" t="s" s="2">
-        <v>333</v>
+        <v>106</v>
       </c>
       <c r="AJ35" t="s" s="2">
         <v>45</v>
@@ -5676,10 +5665,10 @@
         <v>45</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>334</v>
+        <v>45</v>
       </c>
       <c r="AM35" t="s" s="2">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AN35" t="s" s="2">
         <v>45</v>
@@ -5690,39 +5679,43 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
-        <v>45</v>
+        <v>343</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F36" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H36" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I36" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+        <v>345</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>125</v>
+      </c>
       <c r="O36" t="s" s="2">
         <v>45</v>
       </c>
@@ -5770,19 +5763,19 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG36" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH36" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI36" t="s" s="2">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="AJ36" t="s" s="2">
         <v>45</v>
@@ -5794,7 +5787,7 @@
         <v>45</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>340</v>
+        <v>98</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5805,18 +5798,18 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>341</v>
+        <v>347</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F37" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G37" t="s" s="2">
         <v>45</v>
@@ -5828,17 +5821,15 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>100</v>
+        <v>348</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>343</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>128</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" t="s" s="2">
         <v>45</v>
@@ -5887,19 +5878,19 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG37" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>45</v>
+        <v>351</v>
       </c>
       <c r="AI37" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ37" t="s" s="2">
         <v>45</v>
@@ -5908,10 +5899,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>45</v>
+        <v>352</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5922,43 +5913,39 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F38" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G38" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H38" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I38" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>100</v>
+        <v>348</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>347</v>
+        <v>355</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>348</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>129</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
       <c r="O38" t="s" s="2">
         <v>45</v>
       </c>
@@ -6006,19 +5993,19 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG38" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH38" t="s" s="2">
-        <v>45</v>
+        <v>351</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ38" t="s" s="2">
         <v>45</v>
@@ -6027,10 +6014,10 @@
         <v>45</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>45</v>
+        <v>352</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>98</v>
+        <v>357</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6041,7 +6028,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6064,16 +6051,20 @@
         <v>45</v>
       </c>
       <c r="J39" t="s" s="2">
-        <v>351</v>
+        <v>168</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>353</v>
-      </c>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
+        <v>360</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>361</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>362</v>
+      </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
       </c>
@@ -6097,13 +6088,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>45</v>
+        <v>363</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>45</v>
+        <v>364</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6121,7 +6112,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>350</v>
+        <v>358</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6130,7 +6121,7 @@
         <v>55</v>
       </c>
       <c r="AH39" t="s" s="2">
-        <v>354</v>
+        <v>45</v>
       </c>
       <c r="AI39" t="s" s="2">
         <v>67</v>
@@ -6139,13 +6130,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>356</v>
+        <v>276</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6156,7 +6147,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6167,7 +6158,7 @@
         <v>43</v>
       </c>
       <c r="F40" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G40" t="s" s="2">
         <v>45</v>
@@ -6179,16 +6170,20 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>351</v>
+        <v>168</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>358</v>
+        <v>368</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
+        <v>369</v>
+      </c>
+      <c r="M40" t="s" s="2">
+        <v>370</v>
+      </c>
+      <c r="N40" t="s" s="2">
+        <v>371</v>
+      </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
       </c>
@@ -6212,13 +6207,13 @@
         <v>45</v>
       </c>
       <c r="W40" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="X40" t="s" s="2">
-        <v>45</v>
+        <v>372</v>
       </c>
       <c r="Y40" t="s" s="2">
-        <v>45</v>
+        <v>373</v>
       </c>
       <c r="Z40" t="s" s="2">
         <v>45</v>
@@ -6236,16 +6231,16 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>357</v>
+        <v>367</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG40" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH40" t="s" s="2">
-        <v>354</v>
+        <v>45</v>
       </c>
       <c r="AI40" t="s" s="2">
         <v>67</v>
@@ -6254,13 +6249,13 @@
         <v>45</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>45</v>
+        <v>365</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>355</v>
+        <v>366</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>360</v>
+        <v>276</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6271,7 +6266,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6294,19 +6289,17 @@
         <v>45</v>
       </c>
       <c r="J41" t="s" s="2">
-        <v>172</v>
+        <v>375</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>362</v>
+        <v>376</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>363</v>
-      </c>
-      <c r="M41" t="s" s="2">
-        <v>364</v>
-      </c>
+        <v>377</v>
+      </c>
+      <c r="M41" s="2"/>
       <c r="N41" t="s" s="2">
-        <v>365</v>
+        <v>378</v>
       </c>
       <c r="O41" t="s" s="2">
         <v>45</v>
@@ -6331,13 +6324,13 @@
         <v>45</v>
       </c>
       <c r="W41" t="s" s="2">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>366</v>
+        <v>45</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>367</v>
+        <v>45</v>
       </c>
       <c r="Z41" t="s" s="2">
         <v>45</v>
@@ -6355,7 +6348,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>361</v>
+        <v>374</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6373,13 +6366,13 @@
         <v>45</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>368</v>
+        <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>369</v>
+        <v>45</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>279</v>
+        <v>379</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6390,7 +6383,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6401,7 +6394,7 @@
         <v>43</v>
       </c>
       <c r="F42" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G42" t="s" s="2">
         <v>45</v>
@@ -6413,20 +6406,16 @@
         <v>45</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>172</v>
+        <v>57</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>371</v>
+        <v>381</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>372</v>
-      </c>
-      <c r="M42" t="s" s="2">
-        <v>373</v>
-      </c>
-      <c r="N42" t="s" s="2">
-        <v>374</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
         <v>45</v>
       </c>
@@ -6450,13 +6439,13 @@
         <v>45</v>
       </c>
       <c r="W42" t="s" s="2">
-        <v>293</v>
+        <v>45</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>375</v>
+        <v>45</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>376</v>
+        <v>45</v>
       </c>
       <c r="Z42" t="s" s="2">
         <v>45</v>
@@ -6474,13 +6463,13 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG42" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH42" t="s" s="2">
         <v>45</v>
@@ -6492,13 +6481,13 @@
         <v>45</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>368</v>
+        <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>369</v>
+        <v>352</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>279</v>
+        <v>383</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6509,7 +6498,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6520,7 +6509,7 @@
         <v>43</v>
       </c>
       <c r="F43" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G43" t="s" s="2">
         <v>45</v>
@@ -6529,21 +6518,21 @@
         <v>45</v>
       </c>
       <c r="I43" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>380</v>
-      </c>
-      <c r="M43" s="2"/>
-      <c r="N43" t="s" s="2">
-        <v>381</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="M43" t="s" s="2">
+        <v>388</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
         <v>45</v>
       </c>
@@ -6591,13 +6580,13 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG43" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH43" t="s" s="2">
         <v>45</v>
@@ -6612,10 +6601,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>45</v>
+        <v>389</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>382</v>
+        <v>390</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6626,7 +6615,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6637,7 +6626,7 @@
         <v>43</v>
       </c>
       <c r="F44" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G44" t="s" s="2">
         <v>45</v>
@@ -6646,18 +6635,20 @@
         <v>45</v>
       </c>
       <c r="I44" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>57</v>
+        <v>392</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>385</v>
-      </c>
-      <c r="M44" s="2"/>
+        <v>394</v>
+      </c>
+      <c r="M44" t="s" s="2">
+        <v>395</v>
+      </c>
       <c r="N44" s="2"/>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -6706,13 +6697,13 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>383</v>
+        <v>391</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG44" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH44" t="s" s="2">
         <v>45</v>
@@ -6727,10 +6718,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>355</v>
+        <v>389</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>386</v>
+        <v>396</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6741,7 +6732,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6764,18 +6755,20 @@
         <v>56</v>
       </c>
       <c r="J45" t="s" s="2">
-        <v>388</v>
+        <v>325</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>391</v>
-      </c>
-      <c r="N45" s="2"/>
+        <v>400</v>
+      </c>
+      <c r="N45" t="s" s="2">
+        <v>401</v>
+      </c>
       <c r="O45" t="s" s="2">
         <v>45</v>
       </c>
@@ -6823,7 +6816,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>387</v>
+        <v>397</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6844,10 +6837,10 @@
         <v>45</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>393</v>
+        <v>403</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6858,7 +6851,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>394</v>
+        <v>404</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6869,7 +6862,7 @@
         <v>43</v>
       </c>
       <c r="F46" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G46" t="s" s="2">
         <v>45</v>
@@ -6878,20 +6871,18 @@
         <v>45</v>
       </c>
       <c r="I46" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J46" t="s" s="2">
-        <v>395</v>
+        <v>57</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>396</v>
+        <v>334</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>397</v>
-      </c>
-      <c r="M46" t="s" s="2">
-        <v>398</v>
-      </c>
+        <v>335</v>
+      </c>
+      <c r="M46" s="2"/>
       <c r="N46" s="2"/>
       <c r="O46" t="s" s="2">
         <v>45</v>
@@ -6940,19 +6931,19 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>394</v>
+        <v>336</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG46" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH46" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI46" t="s" s="2">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="AJ46" t="s" s="2">
         <v>45</v>
@@ -6961,10 +6952,10 @@
         <v>45</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>392</v>
+        <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>399</v>
+        <v>337</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6975,11 +6966,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>45</v>
+        <v>121</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6995,23 +6986,21 @@
         <v>45</v>
       </c>
       <c r="I47" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J47" t="s" s="2">
-        <v>328</v>
+        <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>401</v>
+        <v>339</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>402</v>
+        <v>340</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>403</v>
-      </c>
-      <c r="N47" t="s" s="2">
-        <v>404</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="N47" s="2"/>
       <c r="O47" t="s" s="2">
         <v>45</v>
       </c>
@@ -7059,7 +7048,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>400</v>
+        <v>341</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7071,7 +7060,7 @@
         <v>45</v>
       </c>
       <c r="AI47" t="s" s="2">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="AJ47" t="s" s="2">
         <v>45</v>
@@ -7080,10 +7069,10 @@
         <v>45</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>405</v>
+        <v>45</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>406</v>
+        <v>337</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>45</v>
@@ -7094,39 +7083,43 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
-        <v>45</v>
+        <v>343</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F48" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H48" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="I48" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J48" t="s" s="2">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>338</v>
-      </c>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
+        <v>345</v>
+      </c>
+      <c r="M48" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="N48" t="s" s="2">
+        <v>125</v>
+      </c>
       <c r="O48" t="s" s="2">
         <v>45</v>
       </c>
@@ -7174,19 +7167,19 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG48" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH48" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI48" t="s" s="2">
-        <v>45</v>
+        <v>106</v>
       </c>
       <c r="AJ48" t="s" s="2">
         <v>45</v>
@@ -7198,7 +7191,7 @@
         <v>45</v>
       </c>
       <c r="AM48" t="s" s="2">
-        <v>340</v>
+        <v>98</v>
       </c>
       <c r="AN48" t="s" s="2">
         <v>45</v>
@@ -7209,18 +7202,18 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
-        <v>125</v>
+        <v>45</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="F49" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G49" t="s" s="2">
         <v>45</v>
@@ -7229,21 +7222,23 @@
         <v>45</v>
       </c>
       <c r="I49" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>100</v>
+        <v>168</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>342</v>
+        <v>408</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>343</v>
+        <v>409</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="N49" s="2"/>
+        <v>410</v>
+      </c>
+      <c r="N49" t="s" s="2">
+        <v>182</v>
+      </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
       </c>
@@ -7267,13 +7262,13 @@
         <v>45</v>
       </c>
       <c r="W49" t="s" s="2">
-        <v>45</v>
+        <v>290</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>45</v>
+        <v>411</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>45</v>
+        <v>412</v>
       </c>
       <c r="Z49" t="s" s="2">
         <v>45</v>
@@ -7291,34 +7286,34 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>344</v>
+        <v>407</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AG49" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI49" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>45</v>
+        <v>413</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>45</v>
+        <v>186</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>340</v>
+        <v>187</v>
       </c>
       <c r="AN49" t="s" s="2">
-        <v>45</v>
+        <v>188</v>
       </c>
       <c r="AO49" t="s" s="2">
         <v>45</v>
@@ -7326,42 +7321,42 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
-        <v>346</v>
+        <v>45</v>
       </c>
       <c r="D50" s="2"/>
       <c r="E50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F50" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="G50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="H50" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="I50" t="s" s="2">
         <v>56</v>
       </c>
       <c r="J50" t="s" s="2">
-        <v>100</v>
+        <v>246</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>347</v>
+        <v>415</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>348</v>
+        <v>248</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>128</v>
+        <v>416</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>129</v>
+        <v>250</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7386,13 +7381,13 @@
         <v>45</v>
       </c>
       <c r="W50" t="s" s="2">
-        <v>45</v>
+        <v>159</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>45</v>
+        <v>417</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>45</v>
+        <v>183</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7410,42 +7405,42 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>349</v>
+        <v>414</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG50" t="s" s="2">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="AJ50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>45</v>
+        <v>418</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>45</v>
+        <v>253</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>98</v>
+        <v>254</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO50" t="s" s="2">
-        <v>45</v>
+        <v>255</v>
       </c>
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7453,7 +7448,7 @@
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="F51" t="s" s="2">
         <v>55</v>
@@ -7465,22 +7460,22 @@
         <v>45</v>
       </c>
       <c r="I51" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J51" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>186</v>
+        <v>260</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7505,13 +7500,13 @@
         <v>45</v>
       </c>
       <c r="W51" t="s" s="2">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>414</v>
+        <v>262</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>415</v>
+        <v>263</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7529,16 +7524,16 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>55</v>
       </c>
       <c r="AH51" t="s" s="2">
-        <v>45</v>
+        <v>264</v>
       </c>
       <c r="AI51" t="s" s="2">
         <v>67</v>
@@ -7547,16 +7542,16 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>416</v>
+        <v>45</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>190</v>
+        <v>98</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>191</v>
+        <v>265</v>
       </c>
       <c r="AN51" t="s" s="2">
-        <v>192</v>
+        <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
         <v>45</v>
@@ -7564,18 +7559,18 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
-        <v>45</v>
+        <v>267</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="F52" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G52" t="s" s="2">
         <v>45</v>
@@ -7584,22 +7579,22 @@
         <v>45</v>
       </c>
       <c r="I52" t="s" s="2">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J52" t="s" s="2">
-        <v>418</v>
+        <v>168</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>419</v>
+        <v>268</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>251</v>
+        <v>269</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>420</v>
+        <v>270</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>253</v>
+        <v>271</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7624,13 +7619,13 @@
         <v>45</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>45</v>
+        <v>261</v>
       </c>
       <c r="X52" t="s" s="2">
-        <v>45</v>
+        <v>272</v>
       </c>
       <c r="Y52" t="s" s="2">
-        <v>45</v>
+        <v>273</v>
       </c>
       <c r="Z52" t="s" s="2">
         <v>45</v>
@@ -7648,13 +7643,13 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>417</v>
+        <v>423</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG52" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH52" t="s" s="2">
         <v>45</v>
@@ -7666,24 +7661,24 @@
         <v>45</v>
       </c>
       <c r="AK52" t="s" s="2">
-        <v>421</v>
+        <v>274</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>256</v>
+        <v>275</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>257</v>
+        <v>276</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>258</v>
+        <v>277</v>
       </c>
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" t="s" s="2">
@@ -7694,7 +7689,7 @@
         <v>43</v>
       </c>
       <c r="F53" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="G53" t="s" s="2">
         <v>45</v>
@@ -7706,19 +7701,19 @@
         <v>45</v>
       </c>
       <c r="J53" t="s" s="2">
-        <v>172</v>
+        <v>45</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>425</v>
+        <v>328</v>
       </c>
       <c r="N53" t="s" s="2">
-        <v>263</v>
+        <v>329</v>
       </c>
       <c r="O53" t="s" s="2">
         <v>45</v>
@@ -7743,13 +7738,13 @@
         <v>45</v>
       </c>
       <c r="W53" t="s" s="2">
-        <v>264</v>
+        <v>45</v>
       </c>
       <c r="X53" t="s" s="2">
-        <v>265</v>
+        <v>45</v>
       </c>
       <c r="Y53" t="s" s="2">
-        <v>266</v>
+        <v>45</v>
       </c>
       <c r="Z53" t="s" s="2">
         <v>45</v>
@@ -7767,16 +7762,16 @@
         <v>45</v>
       </c>
       <c r="AE53" t="s" s="2">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="AF53" t="s" s="2">
         <v>43</v>
       </c>
       <c r="AG53" t="s" s="2">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="AH53" t="s" s="2">
-        <v>267</v>
+        <v>45</v>
       </c>
       <c r="AI53" t="s" s="2">
         <v>67</v>
@@ -7788,258 +7783,20 @@
         <v>45</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>98</v>
+        <v>331</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>268</v>
+        <v>332</v>
       </c>
       <c r="AN53" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="54" hidden="true">
-      <c r="A54" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" t="s" s="2">
-        <v>270</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J54" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="K54" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="L54" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="M54" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="N54" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="O54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P54" s="2"/>
-      <c r="Q54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W54" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="X54" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="Y54" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="Z54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE54" t="s" s="2">
-        <v>426</v>
-      </c>
-      <c r="AF54" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG54" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI54" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AJ54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK54" t="s" s="2">
-        <v>277</v>
-      </c>
-      <c r="AL54" t="s" s="2">
-        <v>278</v>
-      </c>
-      <c r="AM54" t="s" s="2">
-        <v>279</v>
-      </c>
-      <c r="AN54" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO54" t="s" s="2">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="55" hidden="true">
-      <c r="A55" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="D55" s="2"/>
-      <c r="E55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="F55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="G55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="H55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="I55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="J55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="K55" t="s" s="2">
-        <v>428</v>
-      </c>
-      <c r="L55" t="s" s="2">
-        <v>429</v>
-      </c>
-      <c r="M55" t="s" s="2">
-        <v>331</v>
-      </c>
-      <c r="N55" t="s" s="2">
-        <v>332</v>
-      </c>
-      <c r="O55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="P55" s="2"/>
-      <c r="Q55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="R55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="S55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="T55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="U55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="V55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="W55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="X55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Y55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="Z55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AA55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AB55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AC55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AD55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AE55" t="s" s="2">
-        <v>427</v>
-      </c>
-      <c r="AF55" t="s" s="2">
-        <v>43</v>
-      </c>
-      <c r="AG55" t="s" s="2">
-        <v>44</v>
-      </c>
-      <c r="AH55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AI55" t="s" s="2">
-        <v>67</v>
-      </c>
-      <c r="AJ55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AK55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AL55" t="s" s="2">
-        <v>334</v>
-      </c>
-      <c r="AM55" t="s" s="2">
-        <v>335</v>
-      </c>
-      <c r="AN55" t="s" s="2">
-        <v>45</v>
-      </c>
-      <c r="AO55" t="s" s="2">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO55">
+  <autoFilter ref="A1:AO53">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -8049,7 +7806,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI54">
+  <conditionalFormatting sqref="A2:AI52">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>